<commit_message>
added more unit tests for sprint calendar use case.
</commit_message>
<xml_diff>
--- a/doc/use cases - wpf/present-sprint-calendar/present-sprint-member-calendar-decision-table.xlsx
+++ b/doc/use cases - wpf/present-sprint-calendar/present-sprint-member-calendar-decision-table.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects.pet\VeloCity\repo\doc\use cases - wpf\present-sprint-calendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DF6965-A330-4BF4-8DDC-E25CE11841F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1514D64-1EBF-4221-A6B5-626C44D720FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-240" windowWidth="29040" windowHeight="15720" xr2:uid="{CBEE3761-0821-4C79-935C-5732DFDE0CC9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{CBEE3761-0821-4C79-935C-5732DFDE0CC9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="use case" sheetId="2" r:id="rId1"/>
+    <sheet name="days" sheetId="4" r:id="rId2"/>
+    <sheet name="sprint members" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>selected</t>
   </si>
@@ -47,24 +49,12 @@
     <t>a sprint is selected</t>
   </si>
   <si>
-    <t>current day</t>
-  </si>
-  <si>
-    <t>is a day from the sprint</t>
-  </si>
-  <si>
-    <t>is not a day from the sprint</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
     <t>error</t>
   </si>
   <si>
-    <t>display calendar days for the selected sprint and highlights the current day</t>
-  </si>
-  <si>
     <t xml:space="preserve">display calendar days for the selected sprint </t>
   </si>
   <si>
@@ -77,16 +67,91 @@
     <t>no</t>
   </si>
   <si>
-    <t>display calendar days for the last in progress sprint  and highlights the current day</t>
-  </si>
-  <si>
     <t>display calendar days for the last in progress sprint</t>
   </si>
   <si>
-    <t>no (no in progress sprint)</t>
-  </si>
-  <si>
-    <t>yes (one in progress sprint)</t>
+    <t>sprint in progress</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>prerequisites</t>
+  </si>
+  <si>
+    <t>sprint is selected and present in repository</t>
+  </si>
+  <si>
+    <t>date interval</t>
+  </si>
+  <si>
+    <t>current date</t>
+  </si>
+  <si>
+    <t>during sprint</t>
+  </si>
+  <si>
+    <t>outside sprint</t>
+  </si>
+  <si>
+    <t>sprint members</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>many</t>
+  </si>
+  <si>
+    <t>sprint member vacations</t>
+  </si>
+  <si>
+    <t>one day</t>
+  </si>
+  <si>
+    <t>many days</t>
+  </si>
+  <si>
+    <t>one vacation</t>
+  </si>
+  <si>
+    <t>two vacations same member different day</t>
+  </si>
+  <si>
+    <t>two vacations different members same day</t>
+  </si>
+  <si>
+    <t>two vacations different members different day</t>
+  </si>
+  <si>
+    <t>No day displayed</t>
+  </si>
+  <si>
+    <t>one day displayd and it is current</t>
+  </si>
+  <si>
+    <t>one day displayd and it is not current</t>
+  </si>
+  <si>
+    <t>correct number of days displayed and current one selected correctly</t>
+  </si>
+  <si>
+    <t>correct number of days displayed and none is current</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>sprint is selected, it is present in repository and has a length of 7 days</t>
+  </si>
+  <si>
+    <t>no vacation</t>
   </si>
 </sst>
 </file>
@@ -133,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -150,6 +215,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -160,17 +234,32 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -489,17 +578,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65255CD2-7F83-4308-8D8B-87AD40DBECF2}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C13:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="68.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="22" customWidth="1"/>
     <col min="10" max="10" width="34.7109375" customWidth="1"/>
@@ -511,87 +600,285 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AB2A881-1B05-43DA-9007-1E0A15391691}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="22" customWidth="1"/>
+    <col min="12" max="12" width="34.7109375" customWidth="1"/>
+    <col min="13" max="18" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="5"/>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A2:A6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1B72E6-3FE6-4136-9EDD-8EF02706E70B}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="22" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" customWidth="1"/>
+    <col min="11" max="16" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A5:A7"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>